<commit_message>
test: refactor tests for neighbor app views
</commit_message>
<xml_diff>
--- a/neighbors/tests/fixtures/g2u.xlsx
+++ b/neighbors/tests/fixtures/g2u.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramalb/Documents/kcell/python-projects/rantools-v2/neighbors/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3DACF57-B407-D048-AF31-CBBD0417BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7F8FFD-5D6B-C849-9436-1EC32EBF7308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{E3921240-DE84-F04F-BBBE-3173D1D5272A}"/>
+    <workbookView xWindow="2200" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{E3921240-DE84-F04F-BBBE-3173D1D5272A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>source cell</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>gcell2</t>
+  </si>
+  <si>
+    <t>gcell4</t>
   </si>
 </sst>
 </file>
@@ -112,9 +115,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -152,7 +155,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -258,7 +261,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,7 +403,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86BA06F-FF45-474D-80E2-D65270FA764C}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,6 +475,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>